<commit_message>
Finish PCB; Generate outputs
</commit_message>
<xml_diff>
--- a/BOM/discharge-tsmp-board.xlsx
+++ b/BOM/discharge-tsmp-board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonl\repos\baltic-discharge-tsmp\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24A026A4-2CFA-4783-AA6E-DF8A2AB1A357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAEC62BE-5A36-45A9-A015-A51EC275502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{7FB9034F-2C61-490D-9633-5CF5A649D361}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{E9B6DA3A-ACBD-4321-9970-1366F72F313B}"/>
   </bookViews>
   <sheets>
     <sheet name="discharge-tsmp-board" sheetId="1" r:id="rId1"/>
@@ -601,7 +601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{253DCBE0-F763-4559-BD85-9B2B12AE0B0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE41CC9-0CB5-42C6-BE14-331EB7C77C3B}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>